<commit_message>
Farbcode partial with hexadezimal codes
</commit_message>
<xml_diff>
--- a/wiki/generalHomepagedesign/Farbkatalog.xlsx
+++ b/wiki/generalHomepagedesign/Farbkatalog.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -11,12 +11,12 @@
     <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
     <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>Weiß</t>
   </si>
@@ -100,13 +100,25 @@
   </si>
   <si>
     <t>Farbe</t>
+  </si>
+  <si>
+    <t>#404040</t>
+  </si>
+  <si>
+    <t>#254061</t>
+  </si>
+  <si>
+    <t>#FFCC0</t>
+  </si>
+  <si>
+    <t>#98487</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -318,7 +330,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa-Design">
   <a:themeElements>
     <a:clrScheme name="Larissa">
       <a:dk1>
@@ -392,7 +404,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -427,7 +438,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Larissa">
@@ -603,19 +613,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3:D13"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="42.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:10">
       <c r="B2" s="5" t="s">
         <v>26</v>
       </c>
@@ -642,7 +652,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:10">
       <c r="B3" s="3" t="s">
         <v>16</v>
       </c>
@@ -668,7 +678,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:10">
       <c r="B4" s="3" t="s">
         <v>17</v>
       </c>
@@ -684,6 +694,9 @@
       <c r="F4" s="1">
         <v>0</v>
       </c>
+      <c r="G4" t="s">
+        <v>30</v>
+      </c>
       <c r="H4" s="7">
         <v>34</v>
       </c>
@@ -694,7 +707,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:10">
       <c r="B5" s="3" t="s">
         <v>20</v>
       </c>
@@ -720,7 +733,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:10">
       <c r="B6" s="3" t="s">
         <v>18</v>
       </c>
@@ -746,7 +759,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:10">
       <c r="B7" s="3" t="s">
         <v>19</v>
       </c>
@@ -772,7 +785,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:10">
       <c r="B8" s="3" t="s">
         <v>21</v>
       </c>
@@ -798,7 +811,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:10">
       <c r="B9" s="3" t="s">
         <v>22</v>
       </c>
@@ -814,6 +827,9 @@
       <c r="F9" s="1">
         <v>7</v>
       </c>
+      <c r="G9" t="s">
+        <v>31</v>
+      </c>
       <c r="H9" s="7">
         <v>19</v>
       </c>
@@ -824,7 +840,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:10">
       <c r="B10" s="3" t="s">
         <v>23</v>
       </c>
@@ -840,6 +856,9 @@
       <c r="F10" s="1">
         <v>64</v>
       </c>
+      <c r="G10" t="s">
+        <v>28</v>
+      </c>
       <c r="H10" s="7">
         <v>170</v>
       </c>
@@ -850,7 +869,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:10">
       <c r="B11" s="3" t="s">
         <v>24</v>
       </c>
@@ -866,6 +885,9 @@
       <c r="F11" s="1">
         <v>97</v>
       </c>
+      <c r="G11" t="s">
+        <v>29</v>
+      </c>
       <c r="H11" s="7">
         <v>151</v>
       </c>
@@ -876,7 +898,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:10">
       <c r="B12" s="3" t="s">
         <v>25</v>
       </c>
@@ -902,7 +924,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:10">
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="D13" s="9"/>
@@ -920,24 +942,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>